<commit_message>
Added test data reader utility
</commit_message>
<xml_diff>
--- a/testData/fetchTestData/src/test/java/testData/BankManagerSuite.xlsx
+++ b/testData/fetchTestData/src/test/java/testData/BankManagerSuite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003BF8744\testDevelopement\java\testData\fetchTestData\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4676EF7A-3373-4C4E-BA69-82ED7612D9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DF2F95-C7C2-49B2-8F35-9B0F4FE535B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{E02AE2C5-198C-4168-8096-F19B301D3AFB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>TestCases</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Megha</t>
+  </si>
+  <si>
+    <t>runmode</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,7 +508,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Added test data parameterization code to framework
</commit_message>
<xml_diff>
--- a/testData/fetchTestData/src/test/java/testData/BankManagerSuite.xlsx
+++ b/testData/fetchTestData/src/test/java/testData/BankManagerSuite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\003BF8744\testDevelopement\java\testData\fetchTestData\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DF2F95-C7C2-49B2-8F35-9B0F4FE535B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDE75D8-2E7D-4088-8D13-EA88FA98B205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{E02AE2C5-198C-4168-8096-F19B301D3AFB}"/>
   </bookViews>
@@ -492,13 +492,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394803CE-AD09-458D-A9BC-B0BC182277B0}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>